<commit_message>
Commented Read_layers.R and added package name::before functions
</commit_message>
<xml_diff>
--- a/data/key.xlsx
+++ b/data/key.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitHub\local-reef-threats\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\gitHub\local-reef-pressures\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="66">
   <si>
     <t>OBJECTID</t>
   </si>
@@ -51,21 +51,12 @@
     <t>Region</t>
   </si>
   <si>
-    <t>IHO_SEA</t>
-  </si>
-  <si>
-    <t>TERRITORY</t>
-  </si>
-  <si>
     <t>is.bcu</t>
   </si>
   <si>
     <t>BCU_name</t>
   </si>
   <si>
-    <t>COUNTRY</t>
-  </si>
-  <si>
     <t>grav_NC_raw</t>
   </si>
   <si>
@@ -129,9 +120,6 @@
     <t>tp_thrt</t>
   </si>
   <si>
-    <t>TERRITO</t>
-  </si>
-  <si>
     <t>is_bcu</t>
   </si>
   <si>
@@ -195,9 +183,6 @@
     <t>Name of the BCU</t>
   </si>
   <si>
-    <t>Country of the BCU (can differ from TERRITORY because all reefs in the same BCU are forced to have the same COUNTRY)</t>
-  </si>
-  <si>
     <t>Fishing (untransformed)</t>
   </si>
   <si>
@@ -214,9 +199,6 @@
   </si>
   <si>
     <t>Nitrogen (untransformed)</t>
-  </si>
-  <si>
-    <t>Sovereign country of the EEZ of the reef cell</t>
   </si>
   <si>
     <t>Historical thermal stress (TH)</t>
@@ -1042,10 +1024,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,13 +1039,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1071,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1082,7 +1064,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1090,10 +1072,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1101,10 +1083,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1112,10 +1094,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1123,10 +1105,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1134,10 +1116,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1145,10 +1127,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1156,10 +1138,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1175,7 +1157,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1183,10 +1168,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1194,10 +1179,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1205,10 +1190,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1216,10 +1201,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1227,10 +1212,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1238,10 +1223,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1249,10 +1234,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1260,10 +1245,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1271,10 +1256,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1282,10 +1267,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1296,7 +1281,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1307,7 +1292,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1315,43 +1300,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>